<commit_message>
Add short summary table to convey quickly what the results are
Signed-off-by: Bee Nee Lim <beenee.lim@dolphin.fr>
</commit_message>
<xml_diff>
--- a/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_Freeze_v2.0.0/CV32E40Pv2_waiver_list.xlsx
+++ b/Project-Descriptions-and-Plans/CV32E40Pv2/Milestone-data/RTL_Freeze_v2.0.0/CV32E40Pv2_waiver_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dolphinintegrationfr.sharepoint.com/sites/PANTHER/Documents partages/General/CV32E40P/OpenHW Group/RTL_freeze_v2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="888" documentId="13_ncr:40009_{FA898899-A122-4FBE-A95A-CEA7C721CE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85A49A65-DEC9-49CB-91DA-107C1A777C76}"/>
+  <xr:revisionPtr revIDLastSave="902" documentId="13_ncr:40009_{FA898899-A122-4FBE-A95A-CEA7C721CE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A348691-6086-4B63-AAE9-92817AB613D9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="774" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="774" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" summary" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2241" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="295">
   <si>
     <t>code cov waiver</t>
   </si>
@@ -916,6 +916,18 @@
   </si>
   <si>
     <t>feccondrow 241 5</t>
+  </si>
+  <si>
+    <t>one specific condition (Row17) is unreachable. Proven with Formal.</t>
+  </si>
+  <si>
+    <t>feccondrow 387 17</t>
+  </si>
+  <si>
+    <t>one specific condition (Row15) is unreachable. Proven with Formal.</t>
+  </si>
+  <si>
+    <t>feccondrow 396 15</t>
   </si>
 </sst>
 </file>
@@ -2075,8 +2087,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE9C33C9-2B61-4812-A612-B3493AC2B566}" name="Table364" displayName="Table364" ref="A2:F388" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
-  <autoFilter ref="A2:F388" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE9C33C9-2B61-4812-A612-B3493AC2B566}" name="Table364" displayName="Table364" ref="A2:F390" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+  <autoFilter ref="A2:F390" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{3FAB4C40-A884-4ED7-8B0B-4D0D22987092}" name="Line" dataDxfId="37"/>
     <tableColumn id="3" xr3:uid="{C493823C-8987-43EB-BEA4-D5330431F62E}" name="Code coverage type" dataDxfId="36"/>
@@ -7180,10 +7192,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC713BF-A35D-42F8-93DB-E92222AF1DAF}">
-  <dimension ref="A1:F388"/>
+  <dimension ref="A1:F390"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A370" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D395" sqref="D395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14178,6 +14190,46 @@
       </c>
       <c r="F388" s="1">
         <v>64</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A389" s="1">
+        <v>387</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C389" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D389" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E389" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F389" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A390" s="1">
+        <v>396</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D390" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E390" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F390" s="1">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -19407,6 +19459,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="17" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="254d2fc45a10493323dcacd51be5aaf4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="003ab9e0b5c5bed7880e662758cd0922" ns2:_="" ns3:_="">
     <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
@@ -19655,27 +19727,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cbd820e2-9c8a-4c01-9a9c-6b4c26777899">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51aa521f-7cbd-47c5-afee-4a8147a04eed" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D755283-77AF-467A-8C74-DC8595DDCA72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234FD0E2-0AEF-428D-92BF-35044BB2AB06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{643D8826-8392-4BEE-9D5B-BD3352057639}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19692,29 +19769,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D755283-77AF-467A-8C74-DC8595DDCA72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{234FD0E2-0AEF-428D-92BF-35044BB2AB06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>